<commit_message>
update checklist & add .gitignore
</commit_message>
<xml_diff>
--- a/checklists/redcap_import_checklist.xlsx
+++ b/checklists/redcap_import_checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sifre002/Documents/GitHub/redcap-import/checklists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sifre002/Documents/GitHub/qualtrics-to-redcap/checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13B4E4F-351B-704D-ADBD-331CFB898DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F8A225-FBBB-3F4C-A750-A4E9AA628E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-280" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{A2B9708B-ED12-A04C-B1D5-BAA4CF5080C1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{A2B9708B-ED12-A04C-B1D5-BAA4CF5080C1}"/>
   </bookViews>
   <sheets>
     <sheet name="one offs" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -426,6 +426,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,7 +1037,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,31 +1045,32 @@
     <col min="1" max="1" width="47.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="64.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="22" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>